<commit_message>
Scrum sprint2 tasks and completion of sprint1
</commit_message>
<xml_diff>
--- a/doc/task07/CS2_Task7_Scrum_Setup.xlsx
+++ b/doc/task07/CS2_Task7_Scrum_Setup.xlsx
@@ -8,16 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\EclipseWorkspace2020\ch.bfh.bti7081.s2020.black\doc\task07\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F16829A6-B64B-4703-BF37-D464A8138822}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5200461-C70A-467D-8465-83CEDF346F12}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ProjectTeam" sheetId="3" r:id="rId1"/>
     <sheet name="Product Backlog" sheetId="1" r:id="rId2"/>
     <sheet name="Sprint1 Backlog" sheetId="2" r:id="rId3"/>
-    <sheet name="BurndownChart" sheetId="4" r:id="rId4"/>
-    <sheet name="DropDownItems" sheetId="5" r:id="rId5"/>
+    <sheet name="Sprint2 Backlog" sheetId="6" r:id="rId4"/>
+    <sheet name="Sprint3 Backlog" sheetId="7" r:id="rId5"/>
+    <sheet name="BurndownChart" sheetId="4" r:id="rId6"/>
+    <sheet name="DropDownItems" sheetId="5" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -32,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="522" uniqueCount="165">
   <si>
     <t>Name</t>
   </si>
@@ -418,7 +420,115 @@
     <t>3h</t>
   </si>
   <si>
-    <t>7h</t>
+    <t>Account Login</t>
+  </si>
+  <si>
+    <t>Account SignUp</t>
+  </si>
+  <si>
+    <t>Relate Events to Account</t>
+  </si>
+  <si>
+    <t>Implementation of the login logic with DB connection</t>
+  </si>
+  <si>
+    <t>Account SingUp View</t>
+  </si>
+  <si>
+    <t>Task 08 Persistance</t>
+  </si>
+  <si>
+    <t>Revision and extention of the class diagram to include persistence</t>
+  </si>
+  <si>
+    <t>Implementation of the MyEvent UI Elements</t>
+  </si>
+  <si>
+    <t>Friend Request</t>
+  </si>
+  <si>
+    <t>Add Patient to Event</t>
+  </si>
+  <si>
+    <t>Implementation of the logic to give a relative account the funtionality to add a patient to an event</t>
+  </si>
+  <si>
+    <t>Implementation of the functionality to relate an event with specific accounts</t>
+  </si>
+  <si>
+    <t>Implementation of the sign up logic to create a new account and saving the account into the DB</t>
+  </si>
+  <si>
+    <t>Search / Filter Templates</t>
+  </si>
+  <si>
+    <t>Search Public Events</t>
+  </si>
+  <si>
+    <t>Search Public Events View</t>
+  </si>
+  <si>
+    <t>MVP Refactoring</t>
+  </si>
+  <si>
+    <t>Revision of the UI Elements to match the new functionalities</t>
+  </si>
+  <si>
+    <t>Implementation of the Search Public Events UI elements</t>
+  </si>
+  <si>
+    <t>Implementation of the SingUp UI elements</t>
+  </si>
+  <si>
+    <t>Implementation of the search / filter logic for the event templates with UI elements</t>
+  </si>
+  <si>
+    <t>Implementation of the search logic to find public event executions</t>
+  </si>
+  <si>
+    <t>MainLayout</t>
+  </si>
+  <si>
+    <t>Implementation of the MainLayout elements wich are used for all views</t>
+  </si>
+  <si>
+    <t>Refactoring of several classes to match the MVP pattern</t>
+  </si>
+  <si>
+    <t>ChatView</t>
+  </si>
+  <si>
+    <t>ChatPresenter</t>
+  </si>
+  <si>
+    <t>Chat Persistance</t>
+  </si>
+  <si>
+    <t>Implementation of the Chat UI elements</t>
+  </si>
+  <si>
+    <t>Expantion of the database to save and load chats</t>
+  </si>
+  <si>
+    <t>MyEvents View</t>
+  </si>
+  <si>
+    <t>MyEvents Presenter</t>
+  </si>
+  <si>
+    <t>Implementation of the MyEvents presenter to manage the MyEvents View</t>
+  </si>
+  <si>
+    <t>Implementation of the Chat presenter to manage the ChatView</t>
+  </si>
+  <si>
+    <t>Completition of the event creation functionality</t>
+  </si>
+  <si>
+    <t>UI Revision</t>
+  </si>
+  <si>
+    <t>Implementation of the friend request logic to relate a patient with a relative with UI elements</t>
   </si>
 </sst>
 </file>
@@ -945,7 +1055,7 @@
   <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1243,7 +1353,7 @@
         <v>30</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>31</v>
+        <v>113</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1269,7 +1379,7 @@
         <v>30</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>31</v>
+        <v>113</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="75" x14ac:dyDescent="0.25">
@@ -1321,7 +1431,7 @@
         <v>30</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>31</v>
+        <v>113</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -1365,8 +1475,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:R24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1607,10 +1717,10 @@
         <v>64</v>
       </c>
       <c r="K6" t="s">
-        <v>87</v>
+        <v>64</v>
       </c>
       <c r="L6" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="30" x14ac:dyDescent="0.25">
@@ -1648,7 +1758,7 @@
         <v>127</v>
       </c>
       <c r="L7" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="30" x14ac:dyDescent="0.25">
@@ -1794,10 +1904,10 @@
         <v>44</v>
       </c>
       <c r="J11" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="K11" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="L11" t="s">
         <v>114</v>
@@ -1832,13 +1942,13 @@
         <v>44</v>
       </c>
       <c r="J12" t="s">
-        <v>87</v>
+        <v>30</v>
       </c>
       <c r="K12" t="s">
-        <v>87</v>
+        <v>30</v>
       </c>
       <c r="L12" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="30" x14ac:dyDescent="0.25">
@@ -1949,10 +2059,10 @@
         <v>64</v>
       </c>
       <c r="K15" t="s">
-        <v>87</v>
+        <v>64</v>
       </c>
       <c r="L15" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="45" x14ac:dyDescent="0.25">
@@ -1987,10 +2097,10 @@
         <v>64</v>
       </c>
       <c r="K16" t="s">
-        <v>87</v>
+        <v>64</v>
       </c>
       <c r="L16" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="17" spans="1:18" ht="30" x14ac:dyDescent="0.25">
@@ -2032,8 +2142,43 @@
       </c>
       <c r="R17" s="2"/>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A18" s="8"/>
+    <row r="18" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="11">
+        <v>1.17</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="E18" t="s">
+        <v>95</v>
+      </c>
+      <c r="F18" t="s">
+        <v>86</v>
+      </c>
+      <c r="G18" t="s">
+        <v>85</v>
+      </c>
+      <c r="H18" t="s">
+        <v>51</v>
+      </c>
+      <c r="I18" t="s">
+        <v>44</v>
+      </c>
+      <c r="J18" t="s">
+        <v>44</v>
+      </c>
+      <c r="K18" t="s">
+        <v>44</v>
+      </c>
+      <c r="L18" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" s="8"/>
@@ -2081,15 +2226,1050 @@
           <x14:formula1>
             <xm:f>DropDownItems!$C$2:$C$4</xm:f>
           </x14:formula1>
-          <xm:sqref>H2:H17</xm:sqref>
+          <xm:sqref>H2:H18</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{5F2F6BF4-B7B5-43E9-9B95-F1F2611BDB2F}">
           <x14:formula1>
             <xm:f>DropDownItems!$A$2:$A$5</xm:f>
           </x14:formula1>
+          <xm:sqref>L2:L18</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{9F94FF65-21A0-44F8-A6F4-BB8D1FB46FF1}">
+          <x14:formula1>
+            <xm:f>DropDownItems!$E$2:$E$6</xm:f>
+          </x14:formula1>
+          <xm:sqref>F2:G18</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3053B46C-85E6-4BF8-A03F-734870543094}">
+  <dimension ref="A1:R25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J1" sqref="J1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.28515625" customWidth="1"/>
+    <col min="3" max="3" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="35.7109375" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" customWidth="1"/>
+    <col min="6" max="6" width="10.28515625" customWidth="1"/>
+    <col min="7" max="7" width="9.7109375" customWidth="1"/>
+    <col min="8" max="8" width="8.28515625" customWidth="1"/>
+    <col min="9" max="9" width="7.85546875" customWidth="1"/>
+    <col min="10" max="10" width="9.140625" customWidth="1"/>
+    <col min="11" max="11" width="7.28515625" customWidth="1"/>
+    <col min="12" max="12" width="15.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" s="4" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="9">
+        <v>2.1</v>
+      </c>
+      <c r="B2" s="9">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>128</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="E2" t="s">
+        <v>74</v>
+      </c>
+      <c r="H2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I2" t="s">
+        <v>64</v>
+      </c>
+      <c r="J2" t="s">
+        <v>64</v>
+      </c>
+      <c r="L2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="9">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="B3" s="9">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>129</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="E3" t="s">
+        <v>74</v>
+      </c>
+      <c r="H3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I3" t="s">
+        <v>44</v>
+      </c>
+      <c r="J3" t="s">
+        <v>44</v>
+      </c>
+      <c r="L3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="9">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="B4" s="9">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>132</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="E4" t="s">
+        <v>95</v>
+      </c>
+      <c r="H4" t="s">
+        <v>28</v>
+      </c>
+      <c r="I4" t="s">
+        <v>64</v>
+      </c>
+      <c r="J4" t="s">
+        <v>64</v>
+      </c>
+      <c r="L4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="9">
+        <v>2.4</v>
+      </c>
+      <c r="B5" s="9">
+        <v>2</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="E5" t="s">
+        <v>74</v>
+      </c>
+      <c r="H5" t="s">
+        <v>28</v>
+      </c>
+      <c r="I5" t="s">
+        <v>64</v>
+      </c>
+      <c r="J5" t="s">
+        <v>64</v>
+      </c>
+      <c r="L5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="9">
+        <v>2.5</v>
+      </c>
+      <c r="B6" s="9">
+        <v>2</v>
+      </c>
+      <c r="C6" t="s">
+        <v>158</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="E6" t="s">
+        <v>95</v>
+      </c>
+      <c r="H6" t="s">
+        <v>28</v>
+      </c>
+      <c r="I6" t="s">
+        <v>44</v>
+      </c>
+      <c r="J6" t="s">
+        <v>44</v>
+      </c>
+      <c r="L6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="9">
+        <v>2.6</v>
+      </c>
+      <c r="B7" s="9">
+        <v>2</v>
+      </c>
+      <c r="C7" t="s">
+        <v>159</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="E7" t="s">
+        <v>95</v>
+      </c>
+      <c r="H7" t="s">
+        <v>28</v>
+      </c>
+      <c r="I7" t="s">
+        <v>44</v>
+      </c>
+      <c r="J7" t="s">
+        <v>44</v>
+      </c>
+      <c r="L7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="9">
+        <v>2.7</v>
+      </c>
+      <c r="B8" s="9">
+        <v>2</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="E8" t="s">
+        <v>79</v>
+      </c>
+      <c r="H8" t="s">
+        <v>28</v>
+      </c>
+      <c r="I8" t="s">
+        <v>44</v>
+      </c>
+      <c r="J8" t="s">
+        <v>44</v>
+      </c>
+      <c r="L8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="9">
+        <v>2.8</v>
+      </c>
+      <c r="B9" s="9">
+        <v>2</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="E9" t="s">
+        <v>74</v>
+      </c>
+      <c r="H9" t="s">
+        <v>28</v>
+      </c>
+      <c r="I9" t="s">
+        <v>44</v>
+      </c>
+      <c r="J9" t="s">
+        <v>44</v>
+      </c>
+      <c r="L9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" s="9">
+        <v>2.9</v>
+      </c>
+      <c r="B10" s="9">
+        <v>2</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="E10" t="s">
+        <v>74</v>
+      </c>
+      <c r="H10" t="s">
+        <v>28</v>
+      </c>
+      <c r="I10" t="s">
+        <v>64</v>
+      </c>
+      <c r="J10" t="s">
+        <v>64</v>
+      </c>
+      <c r="L10" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11" s="11">
+        <v>2.1</v>
+      </c>
+      <c r="B11" s="9">
+        <v>2</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="E11" t="s">
+        <v>74</v>
+      </c>
+      <c r="H11" t="s">
+        <v>28</v>
+      </c>
+      <c r="I11" t="s">
+        <v>44</v>
+      </c>
+      <c r="J11" t="s">
+        <v>44</v>
+      </c>
+      <c r="L11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="11">
+        <v>2.11</v>
+      </c>
+      <c r="B12" s="9">
+        <v>2</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="E12" t="s">
+        <v>74</v>
+      </c>
+      <c r="H12" t="s">
+        <v>28</v>
+      </c>
+      <c r="I12" t="s">
+        <v>44</v>
+      </c>
+      <c r="J12" t="s">
+        <v>44</v>
+      </c>
+      <c r="L12" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="11">
+        <v>2.12</v>
+      </c>
+      <c r="B13" s="9">
+        <v>2</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="E13" t="s">
+        <v>95</v>
+      </c>
+      <c r="H13" t="s">
+        <v>28</v>
+      </c>
+      <c r="I13" t="s">
+        <v>64</v>
+      </c>
+      <c r="J13" t="s">
+        <v>64</v>
+      </c>
+      <c r="L13" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="11">
+        <v>2.13</v>
+      </c>
+      <c r="B14" s="9">
+        <v>2</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="E14" t="s">
+        <v>74</v>
+      </c>
+      <c r="H14" t="s">
+        <v>28</v>
+      </c>
+      <c r="I14" t="s">
+        <v>44</v>
+      </c>
+      <c r="J14" t="s">
+        <v>44</v>
+      </c>
+      <c r="L14" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="A15" s="11">
+        <v>2.14</v>
+      </c>
+      <c r="B15" s="9">
+        <v>2</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>162</v>
+      </c>
+      <c r="E15" t="s">
+        <v>74</v>
+      </c>
+      <c r="H15" t="s">
+        <v>28</v>
+      </c>
+      <c r="I15" t="s">
+        <v>44</v>
+      </c>
+      <c r="J15" t="s">
+        <v>44</v>
+      </c>
+      <c r="L15" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="11">
+        <v>2.15</v>
+      </c>
+      <c r="B16" s="9">
+        <v>2</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="E16" t="s">
+        <v>95</v>
+      </c>
+      <c r="H16" t="s">
+        <v>28</v>
+      </c>
+      <c r="I16" t="s">
+        <v>44</v>
+      </c>
+      <c r="J16" t="s">
+        <v>44</v>
+      </c>
+      <c r="L16" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="11">
+        <v>2.16</v>
+      </c>
+      <c r="B17" s="9">
+        <v>2</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="E17" t="s">
+        <v>95</v>
+      </c>
+      <c r="H17" t="s">
+        <v>28</v>
+      </c>
+      <c r="I17" t="s">
+        <v>64</v>
+      </c>
+      <c r="J17" t="s">
+        <v>64</v>
+      </c>
+      <c r="L17" t="s">
+        <v>31</v>
+      </c>
+      <c r="R17" s="2"/>
+    </row>
+    <row r="18" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="11">
+        <v>2.17</v>
+      </c>
+      <c r="B18" s="9">
+        <v>2</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="E18" t="s">
+        <v>95</v>
+      </c>
+      <c r="H18" t="s">
+        <v>28</v>
+      </c>
+      <c r="I18" t="s">
+        <v>64</v>
+      </c>
+      <c r="J18" t="s">
+        <v>64</v>
+      </c>
+      <c r="L18" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="11">
+        <v>2.1800000000000002</v>
+      </c>
+      <c r="B19" s="9">
+        <v>2</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="E19" t="s">
+        <v>79</v>
+      </c>
+      <c r="H19" t="s">
+        <v>28</v>
+      </c>
+      <c r="I19" t="s">
+        <v>64</v>
+      </c>
+      <c r="J19" t="s">
+        <v>64</v>
+      </c>
+      <c r="L19" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A20" s="11"/>
+      <c r="B20" s="9"/>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A21" s="8"/>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A22" s="8"/>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A23" s="8"/>
+      <c r="H23" t="s">
+        <v>103</v>
+      </c>
+      <c r="J23" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A24" s="8"/>
+      <c r="H24" t="s">
+        <v>105</v>
+      </c>
+      <c r="J24" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="H25" t="s">
+        <v>107</v>
+      </c>
+      <c r="J25" t="s">
+        <v>108</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{3A7E971D-1444-4552-8EDA-FA73070EA723}">
+          <x14:formula1>
+            <xm:f>DropDownItems!$A$2:$A$5</xm:f>
+          </x14:formula1>
+          <xm:sqref>L2:L21</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{B73FA877-6BD5-4470-A7FB-70EC6D56447D}">
+          <x14:formula1>
+            <xm:f>DropDownItems!$C$2:$C$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>H2:H21</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{06D92DDF-8263-4490-8EDC-61ED81C363FE}">
+          <x14:formula1>
+            <xm:f>DropDownItems!$E$2:$E$6</xm:f>
+          </x14:formula1>
+          <xm:sqref>F2:G3 F5:G17</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07988B06-0D67-49CD-ADDA-87C2BC5A2B1E}">
+  <dimension ref="A1:R24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.28515625" customWidth="1"/>
+    <col min="3" max="3" width="21.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="35.7109375" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" customWidth="1"/>
+    <col min="6" max="6" width="10.28515625" customWidth="1"/>
+    <col min="7" max="7" width="9.7109375" customWidth="1"/>
+    <col min="8" max="8" width="8.28515625" customWidth="1"/>
+    <col min="9" max="9" width="7.85546875" customWidth="1"/>
+    <col min="10" max="10" width="9.140625" customWidth="1"/>
+    <col min="11" max="11" width="7.28515625" customWidth="1"/>
+    <col min="12" max="12" width="15.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" s="4" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="9">
+        <v>3.1</v>
+      </c>
+      <c r="B2" s="9">
+        <v>3</v>
+      </c>
+      <c r="D2" s="7"/>
+      <c r="H2" t="s">
+        <v>28</v>
+      </c>
+      <c r="L2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="9">
+        <v>3.2</v>
+      </c>
+      <c r="B3" s="9">
+        <v>3</v>
+      </c>
+      <c r="D3" s="7"/>
+      <c r="H3" t="s">
+        <v>28</v>
+      </c>
+      <c r="L3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="9">
+        <v>3.3</v>
+      </c>
+      <c r="B4" s="9">
+        <v>3</v>
+      </c>
+      <c r="D4" s="7"/>
+      <c r="H4" t="s">
+        <v>28</v>
+      </c>
+      <c r="L4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="9">
+        <v>3.4</v>
+      </c>
+      <c r="B5" s="9">
+        <v>3</v>
+      </c>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="H5" t="s">
+        <v>28</v>
+      </c>
+      <c r="L5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="9">
+        <v>3.5</v>
+      </c>
+      <c r="B6" s="9">
+        <v>3</v>
+      </c>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="H6" t="s">
+        <v>28</v>
+      </c>
+      <c r="L6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="9">
+        <v>3.6</v>
+      </c>
+      <c r="B7" s="9">
+        <v>3</v>
+      </c>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="H7" t="s">
+        <v>28</v>
+      </c>
+      <c r="L7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="9">
+        <v>3.7</v>
+      </c>
+      <c r="B8" s="9">
+        <v>3</v>
+      </c>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="H8" t="s">
+        <v>28</v>
+      </c>
+      <c r="L8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="9">
+        <v>3.8</v>
+      </c>
+      <c r="B9" s="9">
+        <v>3</v>
+      </c>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="H9" t="s">
+        <v>28</v>
+      </c>
+      <c r="L9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="9">
+        <v>3.9</v>
+      </c>
+      <c r="B10" s="9">
+        <v>3</v>
+      </c>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="H10" t="s">
+        <v>28</v>
+      </c>
+      <c r="L10" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="11">
+        <v>3.1</v>
+      </c>
+      <c r="B11" s="9">
+        <v>3</v>
+      </c>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+      <c r="H11" t="s">
+        <v>28</v>
+      </c>
+      <c r="L11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="11">
+        <v>3.11</v>
+      </c>
+      <c r="B12" s="9">
+        <v>3</v>
+      </c>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="H12" t="s">
+        <v>28</v>
+      </c>
+      <c r="L12" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="11">
+        <v>3.12</v>
+      </c>
+      <c r="B13" s="9">
+        <v>3</v>
+      </c>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
+      <c r="H13" t="s">
+        <v>28</v>
+      </c>
+      <c r="L13" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" s="11">
+        <v>3.13</v>
+      </c>
+      <c r="B14" s="9">
+        <v>3</v>
+      </c>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+      <c r="H14" t="s">
+        <v>28</v>
+      </c>
+      <c r="L14" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" s="11">
+        <v>3.14</v>
+      </c>
+      <c r="B15" s="9">
+        <v>3</v>
+      </c>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="H15" t="s">
+        <v>28</v>
+      </c>
+      <c r="L15" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" s="11">
+        <v>3.15</v>
+      </c>
+      <c r="B16" s="9">
+        <v>3</v>
+      </c>
+      <c r="C16" s="7"/>
+      <c r="D16" s="7"/>
+      <c r="H16" t="s">
+        <v>28</v>
+      </c>
+      <c r="L16" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A17" s="11">
+        <v>3.16</v>
+      </c>
+      <c r="B17" s="9">
+        <v>3</v>
+      </c>
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
+      <c r="H17" t="s">
+        <v>28</v>
+      </c>
+      <c r="L17" t="s">
+        <v>31</v>
+      </c>
+      <c r="R17" s="2"/>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A18" s="8"/>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A19" s="8"/>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A20" s="8"/>
+      <c r="H20" t="s">
+        <v>103</v>
+      </c>
+      <c r="J20" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A21" s="8"/>
+      <c r="H21" t="s">
+        <v>105</v>
+      </c>
+      <c r="J21" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A22" s="8"/>
+      <c r="H22" t="s">
+        <v>107</v>
+      </c>
+      <c r="J22" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A23" s="8"/>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A24" s="8"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{A8A6DB3C-3CE5-417E-8E48-E3D0CECEADE2}">
+          <x14:formula1>
+            <xm:f>DropDownItems!$C$2:$C$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>H2:H17</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{F19E97BA-967B-4BEB-8222-34BB7F0F3C56}">
+          <x14:formula1>
+            <xm:f>DropDownItems!$A$2:$A$5</xm:f>
+          </x14:formula1>
           <xm:sqref>L2:L17</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{9F94FF65-21A0-44F8-A6F4-BB8D1FB46FF1}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{3B99A309-CE46-4B15-BE6D-FBB54541DB5A}">
           <x14:formula1>
             <xm:f>DropDownItems!$E$2:$E$6</xm:f>
           </x14:formula1>
@@ -2101,7 +3281,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D3"/>
   <sheetViews>
@@ -2164,7 +3344,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12E24CED-B6D4-4C91-8BAC-DBE39BEF1DCA}">
   <dimension ref="A1:E6"/>
   <sheetViews>
@@ -2237,12 +3417,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x0101006893662426E20041B5DC715A07C05AC8" ma:contentTypeVersion="7" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="b2dd552918a14c9092dcd1e32bccf7c1">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="f3d1dfd9-2c46-4740-86be-d7afc8a22601" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b756399ce8dcd2fc94ec9bdc36756f4f" ns2:_="">
     <xsd:import namespace="f3d1dfd9-2c46-4740-86be-d7afc8a22601"/>
@@ -2406,6 +3580,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -2416,22 +3596,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A4E5C092-A32C-40DD-BBA1-C6721C518284}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="f3d1dfd9-2c46-4740-86be-d7afc8a22601"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{84E166B6-C298-4931-8E26-6E515A416A42}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2449,6 +3613,22 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A4E5C092-A32C-40DD-BBA1-C6721C518284}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="f3d1dfd9-2c46-4740-86be-d7afc8a22601"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{34F0FDA0-FE5E-4CAA-B492-C0B61EE14632}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Final Scrum and demo video upload
</commit_message>
<xml_diff>
--- a/doc/task07/CS2_Task7_Scrum_Setup.xlsx
+++ b/doc/task07/CS2_Task7_Scrum_Setup.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\EclipseWorkspace2020\ch.bfh.bti7081.s2020.black\doc\task07\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FA1B3D4-4166-48B3-904D-615B5E12D245}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6C8FABF-56C1-4A75-AFB4-8064DDD27E54}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ProjectTeam" sheetId="3" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="719" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="760" uniqueCount="223">
   <si>
     <t>Name</t>
   </si>
@@ -165,18 +165,9 @@
     <t>4h</t>
   </si>
   <si>
-    <t>Send / accept friend request</t>
-  </si>
-  <si>
-    <t>The user (relative) searches for patients and sends a friend request to a patient.</t>
-  </si>
-  <si>
     <t>Add a patient to an event</t>
   </si>
   <si>
-    <t>The owner of the event adds a patient in his freindlist to the event.</t>
-  </si>
-  <si>
     <t>Mark Event done</t>
   </si>
   <si>
@@ -210,12 +201,6 @@
     <t>Once an event is created, the user uses the chat to communicate with other participants.</t>
   </si>
   <si>
-    <t>Check patient's events / info</t>
-  </si>
-  <si>
-    <t>The user (relative) checks the open events of another user (patient) and can see the patient's general information. Accessible via "search patient" mask on landing page and event creation mask.</t>
-  </si>
-  <si>
     <t>Administration via admin account</t>
   </si>
   <si>
@@ -576,9 +561,6 @@
     <t>Finish the logic to use the chat function in public events</t>
   </si>
   <si>
-    <t>Check patient's events / info View and Presenter</t>
-  </si>
-  <si>
     <t>Implementation og the check patient's event view and presenter logic with interfaces</t>
   </si>
   <si>
@@ -685,6 +667,42 @@
   </si>
   <si>
     <t>GUI</t>
+  </si>
+  <si>
+    <t>9h</t>
+  </si>
+  <si>
+    <t>Check patient's events  View and Presenter</t>
+  </si>
+  <si>
+    <t>37h</t>
+  </si>
+  <si>
+    <t>150h</t>
+  </si>
+  <si>
+    <t>The user (relative) searches for patients and adds the patient as a friend.</t>
+  </si>
+  <si>
+    <t>Add a patient / friend</t>
+  </si>
+  <si>
+    <t>The relative adds a patient in his freindlist to the event.</t>
+  </si>
+  <si>
+    <t>Check patient's events</t>
+  </si>
+  <si>
+    <t>The user (relative) checks the open events of another user (patient). Accessible via "My Events" mask on landing page .</t>
+  </si>
+  <si>
+    <t>Relative LVL</t>
+  </si>
+  <si>
+    <t>Relative gets experience for each done event and has a level</t>
+  </si>
+  <si>
+    <t>20h</t>
   </si>
 </sst>
 </file>
@@ -1114,7 +1132,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1143,7 +1161,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -1154,7 +1172,7 @@
         <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -1210,8 +1228,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1269,13 +1287,13 @@
         <v>29</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1298,10 +1316,10 @@
         <v>35</v>
       </c>
       <c r="G3" s="10" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="60" x14ac:dyDescent="0.25">
@@ -1321,13 +1339,13 @@
         <v>38</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="G4" s="10" t="s">
-        <v>102</v>
+        <v>164</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -1335,10 +1353,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>28</v>
@@ -1347,13 +1365,13 @@
         <v>39</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="G5" s="10" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1373,13 +1391,13 @@
         <v>42</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="G6" s="10" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1387,10 +1405,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>43</v>
+        <v>216</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>44</v>
+        <v>215</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>28</v>
@@ -1402,10 +1420,10 @@
         <v>29</v>
       </c>
       <c r="G7" s="10" t="s">
-        <v>124</v>
+        <v>52</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1413,10 +1431,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>46</v>
+        <v>217</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>28</v>
@@ -1428,10 +1446,10 @@
         <v>42</v>
       </c>
       <c r="G8" s="10" t="s">
-        <v>62</v>
+        <v>119</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="60" x14ac:dyDescent="0.25">
@@ -1439,25 +1457,25 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E9" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="C9" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="E9" s="10" t="s">
-        <v>50</v>
-      </c>
       <c r="F9" s="10" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="G9" s="10" t="s">
-        <v>125</v>
+        <v>222</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1465,25 +1483,25 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E10" s="10" t="s">
         <v>42</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="G10" s="10" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -1491,25 +1509,25 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="F11" s="10" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="G11" s="10" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1517,10 +1535,10 @@
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>34</v>
@@ -1532,21 +1550,21 @@
         <v>29</v>
       </c>
       <c r="G12" s="10" t="s">
-        <v>35</v>
+        <v>211</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>58</v>
+        <v>218</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>59</v>
+        <v>219</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>34</v>
@@ -1558,10 +1576,10 @@
         <v>42</v>
       </c>
       <c r="G13" s="10" t="s">
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>31</v>
+        <v>107</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="60" x14ac:dyDescent="0.25">
@@ -1569,49 +1587,71 @@
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>34</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>62</v>
+        <v>80</v>
       </c>
       <c r="F14" s="10" t="s">
-        <v>62</v>
+        <v>80</v>
       </c>
       <c r="G14" s="10" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C15" s="2"/>
-      <c r="G15" s="10"/>
-      <c r="H15" s="1"/>
+        <v>108</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>14</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="D15" t="s">
+        <v>34</v>
+      </c>
+      <c r="E15" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="F15" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="G15" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
-        <v>63</v>
-      </c>
-      <c r="C16" t="s">
-        <v>64</v>
-      </c>
-      <c r="G16" s="10"/>
       <c r="H16" s="1"/>
     </row>
-    <row r="17" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G17" s="10"/>
-    </row>
-    <row r="18" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>58</v>
+      </c>
+      <c r="C17" t="s">
+        <v>59</v>
+      </c>
+      <c r="G17" s="10" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G18" s="10"/>
     </row>
-    <row r="19" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G19" s="10"/>
     </row>
   </sheetData>
@@ -1630,7 +1670,7 @@
           <x14:formula1>
             <xm:f>DropDownItems!$C$2:$C$4</xm:f>
           </x14:formula1>
-          <xm:sqref>D2:D16</xm:sqref>
+          <xm:sqref>D2:D15 D17</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1642,7 +1682,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:R24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A6" workbookViewId="0">
       <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
@@ -1667,7 +1707,7 @@
         <v>18</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>0</v>
@@ -1676,22 +1716,22 @@
         <v>20</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="H1" s="4" t="s">
         <v>21</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="K1" s="4" t="s">
         <v>24</v>
@@ -1708,34 +1748,34 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="E2" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="F2" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="G2" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="H2" t="s">
         <v>28</v>
       </c>
       <c r="I2" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="J2" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="K2" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="L2" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="45" x14ac:dyDescent="0.25">
@@ -1746,34 +1786,34 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="E3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="F3" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="G3" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="H3" t="s">
         <v>28</v>
       </c>
       <c r="I3" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="J3" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="K3" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="L3" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="30" x14ac:dyDescent="0.25">
@@ -1784,34 +1824,34 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="E4" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="F4" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="G4" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="H4" t="s">
         <v>28</v>
       </c>
       <c r="I4" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="J4" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="K4" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="L4" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="30" x14ac:dyDescent="0.25">
@@ -1822,34 +1862,34 @@
         <v>1</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="E5" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="F5" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="G5" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="H5" t="s">
         <v>28</v>
       </c>
       <c r="I5" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="J5" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="K5" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="L5" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="30" x14ac:dyDescent="0.25">
@@ -1860,34 +1900,34 @@
         <v>1</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="E6" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="F6" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="G6" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="H6" t="s">
         <v>34</v>
       </c>
       <c r="I6" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="J6" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="K6" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="L6" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="30" x14ac:dyDescent="0.25">
@@ -1898,34 +1938,34 @@
         <v>1</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="E7" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="F7" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="G7" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="H7" t="s">
         <v>28</v>
       </c>
       <c r="I7" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="J7" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="K7" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="L7" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="30" x14ac:dyDescent="0.25">
@@ -1936,34 +1976,34 @@
         <v>1</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="E8" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="F8" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="G8" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="H8" t="s">
         <v>28</v>
       </c>
       <c r="I8" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="J8" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="K8" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="L8" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="45" x14ac:dyDescent="0.25">
@@ -1974,34 +2014,34 @@
         <v>1</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="E9" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="F9" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="G9" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="H9" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="I9" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="J9" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="K9" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="L9" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="45" x14ac:dyDescent="0.25">
@@ -2012,34 +2052,34 @@
         <v>1</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="E10" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="F10" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="G10" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="H10" t="s">
         <v>34</v>
       </c>
       <c r="I10" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="J10" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="K10" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="L10" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="30" x14ac:dyDescent="0.25">
@@ -2050,19 +2090,19 @@
         <v>1</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="E11" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="F11" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="G11" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="H11" t="s">
         <v>28</v>
@@ -2071,13 +2111,13 @@
         <v>42</v>
       </c>
       <c r="J11" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="K11" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="L11" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="30" x14ac:dyDescent="0.25">
@@ -2088,19 +2128,19 @@
         <v>1</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="E12" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="F12" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="G12" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="H12" t="s">
         <v>28</v>
@@ -2115,7 +2155,7 @@
         <v>30</v>
       </c>
       <c r="L12" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="30" x14ac:dyDescent="0.25">
@@ -2126,34 +2166,34 @@
         <v>1</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="E13" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="F13" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="G13" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="H13" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="I13" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="J13" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="K13" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="L13" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="30" x14ac:dyDescent="0.25">
@@ -2164,34 +2204,34 @@
         <v>1</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="E14" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="F14" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="G14" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="H14" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="I14" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="J14" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="K14" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="L14" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="45" x14ac:dyDescent="0.25">
@@ -2202,34 +2242,34 @@
         <v>1</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="E15" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="F15" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="G15" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="H15" t="s">
         <v>28</v>
       </c>
       <c r="I15" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="J15" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="K15" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="L15" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="45" x14ac:dyDescent="0.25">
@@ -2240,34 +2280,34 @@
         <v>1</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="E16" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="F16" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="G16" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="H16" t="s">
         <v>28</v>
       </c>
       <c r="I16" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="J16" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="K16" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="L16" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
     </row>
     <row r="17" spans="1:18" ht="30" x14ac:dyDescent="0.25">
@@ -2278,34 +2318,34 @@
         <v>1</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="E17" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="F17" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="G17" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="H17" t="s">
         <v>28</v>
       </c>
       <c r="I17" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="J17" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="K17" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="L17" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="R17" s="2"/>
     </row>
@@ -2317,22 +2357,22 @@
         <v>1</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="E18" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="F18" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="G18" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="H18" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="I18" t="s">
         <v>42</v>
@@ -2344,7 +2384,7 @@
         <v>42</v>
       </c>
       <c r="L18" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
@@ -2353,31 +2393,31 @@
     <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" s="8"/>
       <c r="H20" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="J20" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="K20" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" s="8"/>
       <c r="H21" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="J21" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22" s="8"/>
       <c r="H22" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="J22" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.25">
@@ -2420,7 +2460,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3053B46C-85E6-4BF8-A03F-734870543094}">
   <dimension ref="A1:R25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A9" workbookViewId="0">
       <selection activeCell="N15" sqref="N15"/>
     </sheetView>
   </sheetViews>
@@ -2446,7 +2486,7 @@
         <v>18</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>0</v>
@@ -2455,22 +2495,22 @@
         <v>20</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="H1" s="4" t="s">
         <v>21</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="K1" s="4" t="s">
         <v>24</v>
@@ -2487,34 +2527,34 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="E2" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="F2" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="G2" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="H2" t="s">
         <v>28</v>
       </c>
       <c r="I2" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="J2" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="K2" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="L2" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="45" x14ac:dyDescent="0.25">
@@ -2525,22 +2565,22 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="E3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="F3" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="G3" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="H3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="I3" t="s">
         <v>42</v>
@@ -2552,7 +2592,7 @@
         <v>42</v>
       </c>
       <c r="L3" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="30" x14ac:dyDescent="0.25">
@@ -2563,34 +2603,34 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="E4" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="F4" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="G4" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="H4" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="I4" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="J4" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="K4" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="L4" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="30" x14ac:dyDescent="0.25">
@@ -2601,37 +2641,37 @@
         <v>2</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="E5" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="F5" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="G5" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="H5" t="s">
         <v>28</v>
       </c>
       <c r="I5" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="J5" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="K5" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="L5" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="M5" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="30" x14ac:dyDescent="0.25">
@@ -2642,34 +2682,34 @@
         <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="E6" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="F6" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="G6" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="H6" t="s">
         <v>28</v>
       </c>
       <c r="I6" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="J6" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="K6" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="L6" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="45" x14ac:dyDescent="0.25">
@@ -2680,25 +2720,25 @@
         <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="E7" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="F7" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="G7" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="H7" t="s">
         <v>28</v>
       </c>
       <c r="I7" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="J7" t="s">
         <v>42</v>
@@ -2707,7 +2747,7 @@
         <v>42</v>
       </c>
       <c r="L7" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="30" x14ac:dyDescent="0.25">
@@ -2718,19 +2758,19 @@
         <v>2</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="E8" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="F8" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="G8" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="H8" t="s">
         <v>28</v>
@@ -2745,7 +2785,7 @@
         <v>42</v>
       </c>
       <c r="L8" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="45" x14ac:dyDescent="0.25">
@@ -2756,37 +2796,37 @@
         <v>2</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="E9" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="F9" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="G9" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="H9" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="I9" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="J9" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="K9" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="L9" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="M9" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="45" x14ac:dyDescent="0.25">
@@ -2797,34 +2837,34 @@
         <v>2</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="E10" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="F10" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="G10" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="H10" t="s">
         <v>34</v>
       </c>
       <c r="I10" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="J10" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="K10" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="L10" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="45" x14ac:dyDescent="0.25">
@@ -2835,34 +2875,34 @@
         <v>2</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="E11" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="F11" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="G11" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="H11" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="I11" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="J11" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="K11" t="s">
         <v>30</v>
       </c>
       <c r="L11" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
     </row>
     <row r="12" spans="1:13" ht="45" x14ac:dyDescent="0.25">
@@ -2873,22 +2913,22 @@
         <v>2</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="E12" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="F12" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="G12" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="H12" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="I12" t="s">
         <v>42</v>
@@ -2900,7 +2940,7 @@
         <v>42</v>
       </c>
       <c r="L12" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
     </row>
     <row r="13" spans="1:13" ht="45" x14ac:dyDescent="0.25">
@@ -2911,34 +2951,34 @@
         <v>2</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="E13" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="F13" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="G13" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="H13" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="I13" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="J13" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="K13" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="L13" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
     </row>
     <row r="14" spans="1:13" ht="30" x14ac:dyDescent="0.25">
@@ -2949,34 +2989,34 @@
         <v>2</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="E14" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="F14" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="G14" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="H14" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="I14" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="J14" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="K14" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="L14" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
     </row>
     <row r="15" spans="1:13" ht="30" x14ac:dyDescent="0.25">
@@ -2987,19 +3027,19 @@
         <v>2</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="E15" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="F15" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="G15" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="H15" t="s">
         <v>28</v>
@@ -3008,13 +3048,13 @@
         <v>42</v>
       </c>
       <c r="J15" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="K15" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="L15" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
     </row>
     <row r="16" spans="1:13" ht="45" x14ac:dyDescent="0.25">
@@ -3025,19 +3065,19 @@
         <v>2</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="E16" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="F16" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="G16" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="H16" t="s">
         <v>28</v>
@@ -3052,7 +3092,7 @@
         <v>42</v>
       </c>
       <c r="L16" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
     </row>
     <row r="17" spans="1:18" ht="30" x14ac:dyDescent="0.25">
@@ -3063,34 +3103,34 @@
         <v>2</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="E17" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="F17" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="G17" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="H17" t="s">
         <v>34</v>
       </c>
       <c r="I17" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="J17" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="K17" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="L17" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="R17" s="2"/>
     </row>
@@ -3102,34 +3142,34 @@
         <v>2</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="E18" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="F18" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="G18" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="H18" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="I18" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="J18" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="K18" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="L18" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
     </row>
     <row r="19" spans="1:18" ht="30" x14ac:dyDescent="0.25">
@@ -3140,34 +3180,34 @@
         <v>2</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="E19" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="F19" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="G19" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="H19" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="I19" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="J19" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="K19" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="L19" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
     </row>
     <row r="20" spans="1:18" ht="30" x14ac:dyDescent="0.25">
@@ -3178,34 +3218,34 @@
         <v>2</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="E20" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="F20" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="G20" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="H20" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="I20" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="J20" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="K20" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="L20" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.25">
@@ -3217,30 +3257,30 @@
     <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" s="8"/>
       <c r="H23" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="J23" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="K23" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24" s="8"/>
       <c r="H24" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="J24" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="H25" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="J25" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -3277,8 +3317,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07988B06-0D67-49CD-ADDA-87C2BC5A2B1E}">
   <dimension ref="A1:R25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L22" sqref="L22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3302,7 +3342,7 @@
         <v>18</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>0</v>
@@ -3311,22 +3351,22 @@
         <v>20</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="H1" s="4" t="s">
         <v>21</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="K1" s="4" t="s">
         <v>24</v>
@@ -3343,31 +3383,34 @@
         <v>3</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="E2" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="F2" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="G2" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="H2" t="s">
         <v>28</v>
       </c>
       <c r="I2" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="J2" t="s">
-        <v>62</v>
+        <v>57</v>
+      </c>
+      <c r="K2" t="s">
+        <v>80</v>
       </c>
       <c r="L2" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="60" x14ac:dyDescent="0.25">
@@ -3378,31 +3421,34 @@
         <v>3</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="E3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="F3" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="G3" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="H3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="I3" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="J3" t="s">
-        <v>62</v>
+        <v>57</v>
+      </c>
+      <c r="K3" t="s">
+        <v>57</v>
       </c>
       <c r="L3" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="30" x14ac:dyDescent="0.25">
@@ -3413,34 +3459,34 @@
         <v>3</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="E4" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="F4" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="G4" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="H4" t="s">
         <v>28</v>
       </c>
       <c r="I4" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="J4" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="K4" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="L4" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="45" x14ac:dyDescent="0.25">
@@ -3451,19 +3497,19 @@
         <v>3</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="E5" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="F5" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="G5" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="H5" t="s">
         <v>28</v>
@@ -3474,8 +3520,11 @@
       <c r="J5" t="s">
         <v>42</v>
       </c>
+      <c r="K5" t="s">
+        <v>35</v>
+      </c>
       <c r="L5" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="30" x14ac:dyDescent="0.25">
@@ -3486,31 +3535,34 @@
         <v>3</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="E6" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="F6" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="G6" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="H6" t="s">
         <v>28</v>
       </c>
       <c r="I6" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="J6" t="s">
-        <v>62</v>
+        <v>57</v>
+      </c>
+      <c r="K6" t="s">
+        <v>57</v>
       </c>
       <c r="L6" t="s">
-        <v>31</v>
+        <v>107</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="45" x14ac:dyDescent="0.25">
@@ -3521,31 +3573,34 @@
         <v>3</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>180</v>
+        <v>212</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="E7" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="F7" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="G7" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="H7" t="s">
         <v>34</v>
       </c>
       <c r="I7" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="J7" t="s">
-        <v>62</v>
+        <v>57</v>
+      </c>
+      <c r="K7" t="s">
+        <v>57</v>
       </c>
       <c r="L7" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
@@ -3556,19 +3611,19 @@
         <v>3</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="E8" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="F8" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="G8" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="H8" t="s">
         <v>28</v>
@@ -3579,8 +3634,11 @@
       <c r="J8" t="s">
         <v>42</v>
       </c>
+      <c r="K8" t="s">
+        <v>120</v>
+      </c>
       <c r="L8" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="30" x14ac:dyDescent="0.25">
@@ -3591,31 +3649,34 @@
         <v>3</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="E9" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="F9" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="G9" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="H9" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="I9" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="J9" t="s">
-        <v>85</v>
+        <v>80</v>
+      </c>
+      <c r="K9" t="s">
+        <v>80</v>
       </c>
       <c r="L9" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="45" x14ac:dyDescent="0.25">
@@ -3626,19 +3687,19 @@
         <v>3</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="E10" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="F10" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="G10" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="H10" t="s">
         <v>28</v>
@@ -3649,8 +3710,11 @@
       <c r="J10" t="s">
         <v>42</v>
       </c>
+      <c r="K10" t="s">
+        <v>119</v>
+      </c>
       <c r="L10" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="30" x14ac:dyDescent="0.25">
@@ -3661,34 +3725,34 @@
         <v>3</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="E11" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="F11" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="G11" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="H11" t="s">
         <v>28</v>
       </c>
       <c r="I11" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="J11" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="K11" t="s">
-        <v>85</v>
+        <v>57</v>
       </c>
       <c r="L11" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="30" x14ac:dyDescent="0.25">
@@ -3699,34 +3763,34 @@
         <v>3</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="E12" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="F12" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="G12" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="H12" t="s">
         <v>28</v>
       </c>
       <c r="I12" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="J12" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="K12" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="L12" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="45" x14ac:dyDescent="0.25">
@@ -3737,25 +3801,34 @@
         <v>3</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="E13" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="F13" t="s">
-        <v>83</v>
+        <v>78</v>
+      </c>
+      <c r="G13" t="s">
+        <v>69</v>
       </c>
       <c r="H13" t="s">
         <v>28</v>
       </c>
       <c r="I13" t="s">
-        <v>85</v>
+        <v>80</v>
+      </c>
+      <c r="J13" t="s">
+        <v>80</v>
+      </c>
+      <c r="K13" t="s">
+        <v>57</v>
       </c>
       <c r="L13" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="30" x14ac:dyDescent="0.25">
@@ -3766,25 +3839,34 @@
         <v>3</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="E14" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="F14" t="s">
-        <v>73</v>
+        <v>68</v>
+      </c>
+      <c r="G14" t="s">
+        <v>78</v>
       </c>
       <c r="H14" t="s">
         <v>28</v>
       </c>
       <c r="I14" t="s">
-        <v>85</v>
+        <v>80</v>
+      </c>
+      <c r="J14" t="s">
+        <v>80</v>
+      </c>
+      <c r="K14" t="s">
+        <v>80</v>
       </c>
       <c r="L14" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="30" x14ac:dyDescent="0.25">
@@ -3795,25 +3877,34 @@
         <v>3</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="E15" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="F15" t="s">
-        <v>74</v>
+        <v>69</v>
+      </c>
+      <c r="G15" t="s">
+        <v>68</v>
       </c>
       <c r="H15" t="s">
         <v>28</v>
       </c>
       <c r="I15" t="s">
-        <v>85</v>
+        <v>80</v>
+      </c>
+      <c r="J15" t="s">
+        <v>80</v>
+      </c>
+      <c r="K15" t="s">
+        <v>57</v>
       </c>
       <c r="L15" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="30" x14ac:dyDescent="0.25">
@@ -3824,25 +3915,34 @@
         <v>3</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="E16" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="F16" t="s">
-        <v>84</v>
+        <v>79</v>
+      </c>
+      <c r="G16" t="s">
+        <v>78</v>
       </c>
       <c r="H16" t="s">
         <v>28</v>
       </c>
       <c r="I16" t="s">
-        <v>85</v>
+        <v>80</v>
+      </c>
+      <c r="J16" t="s">
+        <v>80</v>
+      </c>
+      <c r="K16" t="s">
+        <v>80</v>
       </c>
       <c r="L16" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="17" spans="1:18" ht="60" x14ac:dyDescent="0.25">
@@ -3853,113 +3953,149 @@
         <v>3</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="E17" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="F17" t="s">
-        <v>83</v>
+        <v>78</v>
+      </c>
+      <c r="G17" t="s">
+        <v>79</v>
       </c>
       <c r="H17" t="s">
         <v>28</v>
       </c>
       <c r="I17" t="s">
-        <v>85</v>
+        <v>80</v>
+      </c>
+      <c r="J17" t="s">
+        <v>80</v>
+      </c>
+      <c r="K17" t="s">
+        <v>80</v>
       </c>
       <c r="L17" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="R17" s="2"/>
     </row>
     <row r="18" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="B18" s="9">
         <v>3</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="E18" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="F18" t="s">
-        <v>74</v>
+        <v>69</v>
+      </c>
+      <c r="G18" t="s">
+        <v>68</v>
       </c>
       <c r="H18" t="s">
         <v>28</v>
       </c>
       <c r="I18" t="s">
-        <v>85</v>
+        <v>80</v>
+      </c>
+      <c r="J18" t="s">
+        <v>80</v>
+      </c>
+      <c r="K18" t="s">
+        <v>80</v>
       </c>
       <c r="L18" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="B19" s="9">
         <v>3</v>
       </c>
       <c r="C19" s="7" t="s">
+        <v>204</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>205</v>
+      </c>
+      <c r="E19" t="s">
         <v>210</v>
       </c>
-      <c r="D19" s="7" t="s">
-        <v>211</v>
-      </c>
-      <c r="E19" t="s">
-        <v>216</v>
-      </c>
       <c r="F19" t="s">
-        <v>84</v>
+        <v>79</v>
+      </c>
+      <c r="G19" t="s">
+        <v>69</v>
       </c>
       <c r="H19" t="s">
         <v>28</v>
       </c>
       <c r="I19" t="s">
-        <v>85</v>
+        <v>80</v>
+      </c>
+      <c r="J19" t="s">
+        <v>80</v>
+      </c>
+      <c r="K19" t="s">
+        <v>57</v>
       </c>
       <c r="L19" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="20" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="B20" s="9">
         <v>3</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="E20" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="F20" t="s">
-        <v>73</v>
+        <v>68</v>
+      </c>
+      <c r="G20" t="s">
+        <v>79</v>
       </c>
       <c r="H20" t="s">
         <v>28</v>
       </c>
       <c r="I20" t="s">
-        <v>85</v>
+        <v>80</v>
+      </c>
+      <c r="J20" t="s">
+        <v>80</v>
+      </c>
+      <c r="K20" t="s">
+        <v>80</v>
       </c>
       <c r="L20" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.25">
@@ -3971,27 +4107,30 @@
     <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" s="8"/>
       <c r="H23" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="J23" t="s">
-        <v>102</v>
+        <v>97</v>
+      </c>
+      <c r="K23" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24" s="8"/>
       <c r="H24" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="J24" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="H25" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="J25" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -4040,16 +4179,16 @@
   <sheetData>
     <row r="1" spans="1:4" s="5" customFormat="1" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -4107,7 +4246,7 @@
         <v>21</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -4120,37 +4259,37 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="C3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E3" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="C4" t="s">
         <v>34</v>
       </c>
       <c r="E4" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="E5" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E6" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -4159,6 +4298,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x0101006893662426E20041B5DC715A07C05AC8" ma:contentTypeVersion="7" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="b2dd552918a14c9092dcd1e32bccf7c1">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="f3d1dfd9-2c46-4740-86be-d7afc8a22601" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b756399ce8dcd2fc94ec9bdc36756f4f" ns2:_="">
     <xsd:import namespace="f3d1dfd9-2c46-4740-86be-d7afc8a22601"/>
@@ -4322,35 +4476,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{84E166B6-C298-4931-8E26-6E515A416A42}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{34F0FDA0-FE5E-4CAA-B492-C0B61EE14632}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="f3d1dfd9-2c46-4740-86be-d7afc8a22601"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -4372,9 +4501,19 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{34F0FDA0-FE5E-4CAA-B492-C0B61EE14632}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{84E166B6-C298-4931-8E26-6E515A416A42}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="f3d1dfd9-2c46-4740-86be-d7afc8a22601"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>